<commit_message>
Adjusted biomass data correctly
</commit_message>
<xml_diff>
--- a/Raw_data/Bag_data.xlsx
+++ b/Raw_data/Bag_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.uws.edu.au\dfshare\HomesCMB$\90957135\My Documents\ABS_FIRE\ABS_FIRE_MYCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westernsydneyedu-my.sharepoint.com/personal/90957135_westernsydney_edu_au/Documents/ABS_FIRE/ABS_FIRE_MYCO/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A172C58-F8E3-4201-A043-2DC2FA019FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{8A172C58-F8E3-4201-A043-2DC2FA019FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDB9336-6A2C-4E71-BAF1-9474514148C9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{287A2311-EA96-4324-AFF2-2DEC9E1B3BFA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{287A2311-EA96-4324-AFF2-2DEC9E1B3BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="67">
   <si>
     <t>Tube_myc</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Before_root.hyphae</t>
+  </si>
+  <si>
+    <t>added in 1g nut sub to help with down stream</t>
   </si>
 </sst>
 </file>
@@ -648,9 +651,9 @@
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -670,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,7 +687,7 @@
         <v>1.5309999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -698,7 +701,7 @@
         <v>1.704</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -715,7 +718,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -732,7 +735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -746,7 +749,7 @@
         <v>2.984</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -763,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -780,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -794,7 +797,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -811,7 +814,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -825,7 +828,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -839,7 +842,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -856,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -873,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -887,7 +890,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -901,7 +904,7 @@
         <v>3.6560000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -915,7 +918,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -929,7 +932,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -943,7 +946,7 @@
         <v>2.6230000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -960,7 +963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -974,7 +977,7 @@
         <v>2.9449999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -988,7 +991,7 @@
         <v>1.3180000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>1.637</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>4.6669999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>1.371</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>1.6759999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>1.2889999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>1.456</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>0.78800000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>1.143</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>2.1850000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>0.623</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1343,7 +1346,7 @@
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>0.94399999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>1.7869999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>0.216</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>0.25700000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>1.9610000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>1.407</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>1.599</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>2.3159999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>1.5780000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>0.96899999999999997</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>1.2190000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>1.093</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>0.92300000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>2.37</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>0.34300000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1652,7 +1655,7 @@
         <v>1.2070000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>3.6240000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>0.51100000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1728,7 +1731,7 @@
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1759,7 +1762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1776,7 +1779,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1793,7 +1796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>1.5609999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>0.96199999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>0.93899999999999995</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>0.68899999999999995</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>2.5840000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>2.5659999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1950,7 +1953,7 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1981,7 +1984,7 @@
         <v>0.89400000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>0.35499999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2029,7 +2032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>1.617</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>3.3090000000000002</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2132,19 +2135,19 @@
   <dimension ref="A1:O192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6328125" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" customWidth="1"/>
-    <col min="14" max="14" width="8.90625" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45356</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45356</v>
       </c>
@@ -2248,8 +2251,8 @@
       <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="s">
-        <v>30</v>
+      <c r="H3">
+        <v>9</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
@@ -2258,7 +2261,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45356</v>
       </c>
@@ -2287,7 +2290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45356</v>
       </c>
@@ -2309,14 +2312,14 @@
       <c r="G5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
-        <v>30</v>
+      <c r="H5">
+        <v>6</v>
       </c>
       <c r="L5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45356</v>
       </c>
@@ -2348,7 +2351,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45356</v>
       </c>
@@ -2364,12 +2367,18 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
       <c r="G7">
         <v>14.12</v>
       </c>
       <c r="H7">
         <v>11</v>
       </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
       <c r="K7" t="s">
         <v>35</v>
       </c>
@@ -2377,7 +2386,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45356</v>
       </c>
@@ -2409,7 +2418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45356</v>
       </c>
@@ -2431,14 +2440,14 @@
       <c r="G9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
-        <v>30</v>
+      <c r="H9">
+        <v>10</v>
       </c>
       <c r="L9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="4" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="4" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>45356</v>
       </c>
@@ -2473,7 +2482,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>45356</v>
       </c>
@@ -2499,7 +2508,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>45356</v>
       </c>
@@ -2537,7 +2546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45356</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>45356</v>
       </c>
@@ -2607,7 +2616,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>45356</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45356</v>
       </c>
@@ -2671,7 +2680,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45356</v>
       </c>
@@ -2703,7 +2712,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45357</v>
       </c>
@@ -2729,7 +2738,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45357</v>
       </c>
@@ -2752,7 +2761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45357</v>
       </c>
@@ -2781,7 +2790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45357</v>
       </c>
@@ -2807,7 +2816,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45357</v>
       </c>
@@ -2836,7 +2845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45357</v>
       </c>
@@ -2862,7 +2871,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>45357</v>
       </c>
@@ -2891,7 +2900,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>45357</v>
       </c>
@@ -2917,7 +2926,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45357</v>
       </c>
@@ -2946,7 +2955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45357</v>
       </c>
@@ -2972,7 +2981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45357</v>
       </c>
@@ -3004,7 +3013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45357</v>
       </c>
@@ -3033,7 +3042,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45357</v>
       </c>
@@ -3062,7 +3071,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45357</v>
       </c>
@@ -3091,7 +3100,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45357</v>
       </c>
@@ -3123,7 +3132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45357</v>
       </c>
@@ -3155,7 +3164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45357</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45357</v>
       </c>
@@ -3219,7 +3228,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45357</v>
       </c>
@@ -3245,7 +3254,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45357</v>
       </c>
@@ -3264,8 +3273,8 @@
       <c r="G37" t="s">
         <v>30</v>
       </c>
-      <c r="H37" t="s">
-        <v>30</v>
+      <c r="H37">
+        <v>39</v>
       </c>
       <c r="K37" t="s">
         <v>38</v>
@@ -3274,7 +3283,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45357</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45357</v>
       </c>
@@ -3331,14 +3340,14 @@
       <c r="G39" t="s">
         <v>30</v>
       </c>
-      <c r="H39" t="s">
-        <v>30</v>
+      <c r="H39">
+        <v>3</v>
       </c>
       <c r="L39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45357</v>
       </c>
@@ -3370,7 +3379,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45357</v>
       </c>
@@ -3399,7 +3408,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45357</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45357</v>
       </c>
@@ -3460,7 +3469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45357</v>
       </c>
@@ -3492,7 +3501,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45357</v>
       </c>
@@ -3521,7 +3530,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45357</v>
       </c>
@@ -3550,7 +3559,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45357</v>
       </c>
@@ -3573,7 +3582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45357</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45357</v>
       </c>
@@ -3637,7 +3646,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45357</v>
       </c>
@@ -3672,7 +3681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>45357</v>
       </c>
@@ -3701,7 +3710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>45357</v>
       </c>
@@ -3730,7 +3739,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>45357</v>
       </c>
@@ -3752,14 +3761,14 @@
       <c r="G53" t="s">
         <v>30</v>
       </c>
-      <c r="H53" t="s">
-        <v>30</v>
+      <c r="H53">
+        <v>1</v>
       </c>
       <c r="L53" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>45357</v>
       </c>
@@ -3794,7 +3803,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>45357</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>45359</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>45359</v>
       </c>
@@ -3881,7 +3890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>45359</v>
       </c>
@@ -3907,7 +3916,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>45359</v>
       </c>
@@ -3929,8 +3938,8 @@
       <c r="G59" t="s">
         <v>30</v>
       </c>
-      <c r="H59" t="s">
-        <v>30</v>
+      <c r="H59">
+        <v>38</v>
       </c>
       <c r="K59" t="s">
         <v>36</v>
@@ -3939,7 +3948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45359</v>
       </c>
@@ -3965,7 +3974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>45359</v>
       </c>
@@ -3987,14 +3996,14 @@
       <c r="G61" t="s">
         <v>30</v>
       </c>
-      <c r="H61" t="s">
-        <v>30</v>
+      <c r="H61">
+        <v>37</v>
       </c>
       <c r="L61" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>45359</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45359</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="10">
         <v>45359</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10">
         <v>45359</v>
       </c>
@@ -4116,7 +4125,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>45359</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>45359</v>
       </c>
@@ -4165,7 +4174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>45359</v>
       </c>
@@ -4191,7 +4200,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>45359</v>
       </c>
@@ -4214,7 +4223,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>45359</v>
       </c>
@@ -4249,7 +4258,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>45359</v>
       </c>
@@ -4284,7 +4293,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>45359</v>
       </c>
@@ -4313,7 +4322,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>45359</v>
       </c>
@@ -4339,7 +4348,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>45359</v>
       </c>
@@ -4368,7 +4377,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>45359</v>
       </c>
@@ -4394,7 +4403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>45359</v>
       </c>
@@ -4426,7 +4435,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>45359</v>
       </c>
@@ -4452,7 +4461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>45359</v>
       </c>
@@ -4481,7 +4490,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>45359</v>
       </c>
@@ -4507,7 +4516,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45357</v>
       </c>
@@ -4536,7 +4545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>45357</v>
       </c>
@@ -4562,7 +4571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>45357</v>
       </c>
@@ -4588,7 +4597,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>45357</v>
       </c>
@@ -4614,7 +4623,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>45357</v>
       </c>
@@ -4640,7 +4649,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>45357</v>
       </c>
@@ -4663,7 +4672,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>45357</v>
       </c>
@@ -4692,7 +4701,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>45357</v>
       </c>
@@ -4718,7 +4727,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>45357</v>
       </c>
@@ -4744,7 +4753,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>45357</v>
       </c>
@@ -4767,7 +4776,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>45357</v>
       </c>
@@ -4793,7 +4802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>45357</v>
       </c>
@@ -4816,7 +4825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>45357</v>
       </c>
@@ -4842,7 +4851,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>45357</v>
       </c>
@@ -4865,7 +4874,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>45357</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>45357</v>
       </c>
@@ -4914,7 +4923,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>45359</v>
       </c>
@@ -4943,7 +4952,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>45359</v>
       </c>
@@ -4966,7 +4975,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>45359</v>
       </c>
@@ -4992,7 +5001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>45359</v>
       </c>
@@ -5015,7 +5024,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>45359</v>
       </c>
@@ -5041,7 +5050,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>45359</v>
       </c>
@@ -5064,7 +5073,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>45359</v>
       </c>
@@ -5090,7 +5099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="103" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>45359</v>
       </c>
@@ -5113,7 +5122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>45359</v>
       </c>
@@ -5142,7 +5151,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>45359</v>
       </c>
@@ -5168,7 +5177,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>45359</v>
       </c>
@@ -5194,7 +5203,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>45359</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>45357</v>
       </c>
@@ -5243,7 +5252,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>45357</v>
       </c>
@@ -5266,7 +5275,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>45357</v>
       </c>
@@ -5292,7 +5301,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>45357</v>
       </c>
@@ -5318,7 +5327,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>45357</v>
       </c>
@@ -5344,7 +5353,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>45357</v>
       </c>
@@ -5367,7 +5376,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>45357</v>
       </c>
@@ -5393,7 +5402,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>45357</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>45359</v>
       </c>
@@ -5448,7 +5457,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>45359</v>
       </c>
@@ -5471,7 +5480,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>45359</v>
       </c>
@@ -5500,7 +5509,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>45359</v>
       </c>
@@ -5522,8 +5531,8 @@
       <c r="G119" t="s">
         <v>30</v>
       </c>
-      <c r="H119" t="s">
-        <v>30</v>
+      <c r="H119">
+        <v>70</v>
       </c>
       <c r="I119" t="s">
         <v>44</v>
@@ -5532,7 +5541,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>45359</v>
       </c>
@@ -5558,7 +5567,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>45359</v>
       </c>
@@ -5581,7 +5590,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>45359</v>
       </c>
@@ -5607,7 +5616,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>45359</v>
       </c>
@@ -5630,7 +5639,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45359</v>
       </c>
@@ -5656,7 +5665,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>45359</v>
       </c>
@@ -5678,8 +5687,8 @@
       <c r="G125" t="s">
         <v>30</v>
       </c>
-      <c r="H125" t="s">
-        <v>30</v>
+      <c r="H125">
+        <v>64</v>
       </c>
       <c r="I125" t="s">
         <v>38</v>
@@ -5688,7 +5697,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>45359</v>
       </c>
@@ -5714,7 +5723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>45359</v>
       </c>
@@ -5737,7 +5746,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>45359</v>
       </c>
@@ -5763,7 +5772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>45359</v>
       </c>
@@ -5786,7 +5795,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>45359</v>
       </c>
@@ -5812,7 +5821,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>45359</v>
       </c>
@@ -5834,14 +5843,14 @@
       <c r="G131" t="s">
         <v>30</v>
       </c>
-      <c r="H131" t="s">
-        <v>30</v>
+      <c r="H131">
+        <v>71</v>
       </c>
       <c r="L131" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>45359</v>
       </c>
@@ -5867,7 +5876,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>45359</v>
       </c>
@@ -5890,7 +5899,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>45359</v>
       </c>
@@ -5916,7 +5925,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>45359</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>45359</v>
       </c>
@@ -5965,7 +5974,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>45359</v>
       </c>
@@ -5988,7 +5997,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>45359</v>
       </c>
@@ -6014,7 +6023,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>45359</v>
       </c>
@@ -6037,7 +6046,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>45357</v>
       </c>
@@ -6063,7 +6072,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>45357</v>
       </c>
@@ -6086,7 +6095,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>45357</v>
       </c>
@@ -6112,7 +6121,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>45357</v>
       </c>
@@ -6135,7 +6144,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>45359</v>
       </c>
@@ -6161,7 +6170,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>45359</v>
       </c>
@@ -6184,7 +6193,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>45359</v>
       </c>
@@ -6210,7 +6219,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>45359</v>
       </c>
@@ -6239,7 +6248,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>45359</v>
       </c>
@@ -6265,7 +6274,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>45359</v>
       </c>
@@ -6288,7 +6297,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>45359</v>
       </c>
@@ -6317,7 +6326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>45359</v>
       </c>
@@ -6340,7 +6349,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>45359</v>
       </c>
@@ -6366,7 +6375,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>45359</v>
       </c>
@@ -6389,7 +6398,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>45359</v>
       </c>
@@ -6415,7 +6424,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>45359</v>
       </c>
@@ -6438,7 +6447,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>45359</v>
       </c>
@@ -6464,7 +6473,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>45359</v>
       </c>
@@ -6490,7 +6499,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>45359</v>
       </c>
@@ -6519,8 +6528,11 @@
         <v>52</v>
       </c>
       <c r="J158" s="8"/>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L158" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>45359</v>
       </c>
@@ -6536,6 +6548,9 @@
       <c r="E159" t="s">
         <v>28</v>
       </c>
+      <c r="F159">
+        <v>1</v>
+      </c>
       <c r="G159">
         <v>14.656000000000001</v>
       </c>
@@ -6543,7 +6558,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>45359</v>
       </c>
@@ -6569,7 +6584,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>45359</v>
       </c>
@@ -6592,7 +6607,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>45359</v>
       </c>
@@ -6618,7 +6633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>45359</v>
       </c>
@@ -6641,7 +6656,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>45360</v>
       </c>
@@ -6667,7 +6682,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>45360</v>
       </c>
@@ -6690,7 +6705,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>45360</v>
       </c>
@@ -6716,7 +6731,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>45360</v>
       </c>
@@ -6739,7 +6754,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>45360</v>
       </c>
@@ -6765,7 +6780,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>45360</v>
       </c>
@@ -6787,8 +6802,8 @@
       <c r="G169" t="s">
         <v>30</v>
       </c>
-      <c r="H169" t="s">
-        <v>30</v>
+      <c r="H169">
+        <v>89</v>
       </c>
       <c r="I169" t="s">
         <v>38</v>
@@ -6797,7 +6812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>45360</v>
       </c>
@@ -6823,7 +6838,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>45360</v>
       </c>
@@ -6849,7 +6864,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>45357</v>
       </c>
@@ -6875,7 +6890,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>45357</v>
       </c>
@@ -6898,7 +6913,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>45357</v>
       </c>
@@ -6927,7 +6942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>45357</v>
       </c>
@@ -6953,7 +6968,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>45360</v>
       </c>
@@ -6979,7 +6994,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>45360</v>
       </c>
@@ -7002,7 +7017,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>45360</v>
       </c>
@@ -7025,13 +7040,13 @@
         <v>13.01</v>
       </c>
       <c r="H178">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="N178" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>45360</v>
       </c>
@@ -7051,13 +7066,13 @@
         <v>12.026</v>
       </c>
       <c r="H179">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="K179" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>45360</v>
       </c>
@@ -7083,7 +7098,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>45360</v>
       </c>
@@ -7106,7 +7121,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>45360</v>
       </c>
@@ -7132,7 +7147,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>45360</v>
       </c>
@@ -7158,7 +7173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>45359</v>
       </c>
@@ -7187,8 +7202,11 @@
         <v>52</v>
       </c>
       <c r="J184" s="8"/>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="L184" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>45359</v>
       </c>
@@ -7204,6 +7222,9 @@
       <c r="E185" t="s">
         <v>28</v>
       </c>
+      <c r="F185">
+        <v>1</v>
+      </c>
       <c r="G185">
         <v>14.474</v>
       </c>
@@ -7214,7 +7235,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>45359</v>
       </c>
@@ -7240,7 +7261,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>45359</v>
       </c>
@@ -7263,7 +7284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>45359</v>
       </c>
@@ -7289,7 +7310,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>45359</v>
       </c>
@@ -7312,7 +7333,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>45359</v>
       </c>
@@ -7338,7 +7359,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>45359</v>
       </c>
@@ -7364,7 +7385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192" s="1"/>
     </row>
   </sheetData>

</xml_diff>